<commit_message>
Updated UDI GMDN fields.
</commit_message>
<xml_diff>
--- a/static/fields/deviceudi_reference.xlsx
+++ b/static/fields/deviceudi_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26803"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7F77005D-4821-4AE4-A6AB-5988924918E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A78CF20-28BE-4B0D-8584-D4C371DD6372}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3830A780-073A-4AEF-96B5-7D9CC2E92E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1003" yWindow="0" windowWidth="23455" windowHeight="12485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="151">
   <si>
     <t>Section</t>
   </si>
@@ -466,18 +466,40 @@
     <t>GMDN Terms</t>
   </si>
   <si>
+    <t>gmdn_terms.code</t>
+  </si>
+  <si>
+    <t>GMDN Preferred Term Code of the common device type associated with the FDA PT Code.</t>
+  </si>
+  <si>
     <t>gmdn_terms.name</t>
   </si>
   <si>
-    <t>Firm name of owner operator.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+    <t>Name of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
   </si>
   <si>
     <t>gmdn_terms.definition</t>
   </si>
   <si>
-    <t>Official correspondent first name.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+    <t>Definition of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
+  </si>
+  <si>
+    <t>gmdn_terms.implantable</t>
+  </si>
+  <si>
+    <t>GMDN Implantable flag.
+Value is one of the following
+true = true
+false = false</t>
+  </si>
+  <si>
+    <t>gmdn_terms.code_status</t>
+  </si>
+  <si>
+    <t>GMDN Term Status, Active or Obsolete.
+Value is one of the following
+Active = Active
+Obsolete = Obsolete</t>
   </si>
   <si>
     <t>Premarket Submissions</t>
@@ -962,159 +984,259 @@
     </xf>
   </cellXfs>
   <cellStyles count="273">
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
@@ -1122,118 +1244,18 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1574,10 +1596,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
@@ -1933,7 +1955,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="79.150000000000006">
+    <row r="36" spans="1:4" ht="81">
       <c r="B36" s="4" t="s">
         <v>68</v>
       </c>
@@ -2195,7 +2217,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="47.45">
+    <row r="56" spans="1:4" ht="16.5">
       <c r="A56" s="3" t="s">
         <v>110</v>
       </c>
@@ -2209,7 +2231,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="47.45">
+    <row r="57" spans="1:4" ht="16.5">
       <c r="A57" s="3" t="s">
         <v>110</v>
       </c>
@@ -2223,65 +2245,68 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" ht="16.5">
       <c r="A58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="5" t="s">
+    </row>
+    <row r="59" spans="1:4" ht="81">
+      <c r="A59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="5" t="s">
+    </row>
+    <row r="60" spans="1:4" ht="81">
+      <c r="A60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="119.85" customHeight="1">
-      <c r="A60" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="5" t="s">
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="47.45">
-      <c r="A61" s="3" t="s">
+      <c r="B61" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="5" t="s">
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="47.45">
-      <c r="A62" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
@@ -2290,11 +2315,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="47.45">
+    <row r="63" spans="1:4" ht="119.85" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -2306,24 +2331,21 @@
     </row>
     <row r="64" spans="1:4" ht="47.45">
       <c r="A64" s="3" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="47.45">
+      <c r="A65" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>5</v>
@@ -2332,11 +2354,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" ht="47.45">
       <c r="A66" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>132</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -2346,51 +2368,51 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="142.5">
+    <row r="67" spans="1:4" ht="47.45">
       <c r="A67" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="5" t="s">
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="47.45">
-      <c r="A68" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="3" t="s">
+    </row>
+    <row r="70" spans="1:4" ht="142.5">
+      <c r="A70" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="63.4">
-      <c r="A70" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>141</v>
@@ -2404,18 +2426,61 @@
     </row>
     <row r="71" spans="1:4" ht="47.45">
       <c r="A71" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>143</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>144</v>
       </c>
     </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="63.4">
+      <c r="A73" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="47.45">
+      <c r="A74" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fda 470 udi gmdn updates (#251)
* Updated UDI GMDN fields.

* Updated master_fields.yaml
</commit_message>
<xml_diff>
--- a/static/fields/deviceudi_reference.xlsx
+++ b/static/fields/deviceudi_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26803"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7F77005D-4821-4AE4-A6AB-5988924918E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A78CF20-28BE-4B0D-8584-D4C371DD6372}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3830A780-073A-4AEF-96B5-7D9CC2E92E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1003" yWindow="0" windowWidth="23455" windowHeight="12485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="151">
   <si>
     <t>Section</t>
   </si>
@@ -466,18 +466,40 @@
     <t>GMDN Terms</t>
   </si>
   <si>
+    <t>gmdn_terms.code</t>
+  </si>
+  <si>
+    <t>GMDN Preferred Term Code of the common device type associated with the FDA PT Code.</t>
+  </si>
+  <si>
     <t>gmdn_terms.name</t>
   </si>
   <si>
-    <t>Firm name of owner operator.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+    <t>Name of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
   </si>
   <si>
     <t>gmdn_terms.definition</t>
   </si>
   <si>
-    <t>Official correspondent first name.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+    <t>Definition of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
+  </si>
+  <si>
+    <t>gmdn_terms.implantable</t>
+  </si>
+  <si>
+    <t>GMDN Implantable flag.
+Value is one of the following
+true = true
+false = false</t>
+  </si>
+  <si>
+    <t>gmdn_terms.code_status</t>
+  </si>
+  <si>
+    <t>GMDN Term Status, Active or Obsolete.
+Value is one of the following
+Active = Active
+Obsolete = Obsolete</t>
   </si>
   <si>
     <t>Premarket Submissions</t>
@@ -962,159 +984,259 @@
     </xf>
   </cellXfs>
   <cellStyles count="273">
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
@@ -1122,118 +1244,18 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1574,10 +1596,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
@@ -1933,7 +1955,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="79.150000000000006">
+    <row r="36" spans="1:4" ht="81">
       <c r="B36" s="4" t="s">
         <v>68</v>
       </c>
@@ -2195,7 +2217,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="47.45">
+    <row r="56" spans="1:4" ht="16.5">
       <c r="A56" s="3" t="s">
         <v>110</v>
       </c>
@@ -2209,7 +2231,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="47.45">
+    <row r="57" spans="1:4" ht="16.5">
       <c r="A57" s="3" t="s">
         <v>110</v>
       </c>
@@ -2223,65 +2245,68 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" ht="16.5">
       <c r="A58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="5" t="s">
+    </row>
+    <row r="59" spans="1:4" ht="81">
+      <c r="A59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="5" t="s">
+    </row>
+    <row r="60" spans="1:4" ht="81">
+      <c r="A60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="119.85" customHeight="1">
-      <c r="A60" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="5" t="s">
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="47.45">
-      <c r="A61" s="3" t="s">
+      <c r="B61" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="5" t="s">
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="47.45">
-      <c r="A62" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
@@ -2290,11 +2315,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="47.45">
+    <row r="63" spans="1:4" ht="119.85" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -2306,24 +2331,21 @@
     </row>
     <row r="64" spans="1:4" ht="47.45">
       <c r="A64" s="3" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="47.45">
+      <c r="A65" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>5</v>
@@ -2332,11 +2354,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" ht="47.45">
       <c r="A66" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>132</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -2346,51 +2368,51 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="142.5">
+    <row r="67" spans="1:4" ht="47.45">
       <c r="A67" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="5" t="s">
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="47.45">
-      <c r="A68" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="3" t="s">
+    </row>
+    <row r="70" spans="1:4" ht="142.5">
+      <c r="A70" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="63.4">
-      <c r="A70" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>141</v>
@@ -2404,18 +2426,61 @@
     </row>
     <row r="71" spans="1:4" ht="47.45">
       <c r="A71" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>143</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>144</v>
       </c>
     </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="63.4">
+      <c r="A73" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="47.45">
+      <c r="A74" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
UDI Searchable Fields Reference Document updated
</commit_message>
<xml_diff>
--- a/static/fields/deviceudi_reference.xlsx
+++ b/static/fields/deviceudi_reference.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/59009_icf_com/Documents/Documents/open-fda/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3830A780-073A-4AEF-96B5-7D9CC2E92E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{3830A780-073A-4AEF-96B5-7D9CC2E92E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42600800-3E0E-4158-B7EE-FB60B1E866C2}"/>
   <bookViews>
-    <workbookView xWindow="1003" yWindow="0" windowWidth="23455" windowHeight="12485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_udi_fields" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">device_udi_fields!$C$80</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -535,38 +538,16 @@
     <t>storage.high.value</t>
   </si>
   <si>
-    <t>Official correspondent last name.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>Official correspondent middle initial.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
     <t>storage.low.value</t>
   </si>
   <si>
-    <t>Official correspondent phone number.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.eprocessed and reused.</t>
-  </si>
-  <si>
     <t>storage.low.unit</t>
   </si>
   <si>
-    <t>Official correspondent company name (if different from owner operator company name).
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
     <t>storage.special_conditions</t>
   </si>
   <si>
-    <t>First line of address for owner operator.</t>
-  </si>
-  <si>
     <t>storage.type</t>
-  </si>
-  <si>
-    <t>Second line of address for owner operator.</t>
   </si>
   <si>
     <t>OpenFDA fields</t>
@@ -610,12 +591,39 @@
   <si>
     <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
   </si>
+  <si>
+    <t>Indicates the high value for storage and handling requirements.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>The low value unit of measures associated with the storage and handling conditions.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.eprocessed and reused.</t>
+  </si>
+  <si>
+    <t>Indicates the low value for storage and handling requirements.Value is one of the following
+Degrees Celsius = Degrees Celsius
+Degrees Fahrenheit = Degrees Fahrenheit
+Degrees Kelvin = Degrees Kelvin
+Kilo Pascal = Kilo Pascal
+Percent (%) Relative Humidity, Millibar = Percent (%) Relative Humidity,Millibar
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized</t>
+  </si>
+  <si>
+    <t>Indicated any special storage requirements for the device.</t>
+  </si>
+  <si>
+    <t>Indicates storage and handling requirements for the device inclusing temperature, humidity, and atmospheric pressure.</t>
+  </si>
+  <si>
+    <t>The high value unit of measure associated with the storage and handling conditions.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -669,7 +677,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -677,6 +685,154 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -953,14 +1109,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -970,17 +1120,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="273">
@@ -1269,6 +1455,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1596,895 +1786,956 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B70" sqref="A34:D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="3"/>
+    <col min="1" max="1" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="118.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="79.150000000000006">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.45">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:4" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14"/>
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.7">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14"/>
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="110.85">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.45">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14"/>
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14"/>
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="126.75">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:4" ht="145.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="110.85">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:4" ht="133.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14"/>
+      <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="126.75">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:4" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="110.85">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:4" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="110.85">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="110.85">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:4" ht="131.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="79.150000000000006">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:4" ht="98" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="95.1">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="95.1">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:4" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="110.85">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:4" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="14"/>
+      <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="126.75">
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:4" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="79.150000000000006">
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:4" ht="98.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="79.150000000000006">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14"/>
+      <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="79.150000000000006">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:4" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="B22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="79.150000000000006">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14"/>
+      <c r="B23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="31.7">
-      <c r="B24" s="4" t="s">
+    <row r="24" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="14"/>
+      <c r="B24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="158.44999999999999">
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="1:4" ht="175" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14"/>
+      <c r="B25" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="31.7">
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="1:4" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14"/>
+      <c r="B26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="4" t="s">
+    <row r="27" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14"/>
+      <c r="B28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="4" t="s">
+    <row r="29" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="14"/>
+      <c r="B30" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="14"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="14"/>
+      <c r="B32" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="43.7" customHeight="1">
-      <c r="B34" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="14"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="1:4" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="14"/>
+      <c r="B34" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="95.1">
-      <c r="B35" s="4" t="s">
+    <row r="35" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+      <c r="A35" s="14"/>
+      <c r="B35" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="81">
-      <c r="B36" s="4" t="s">
+    <row r="36" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="14"/>
+      <c r="B36" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="79.150000000000006">
-      <c r="B37" s="4" t="s">
+    <row r="37" spans="1:4" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="14"/>
+      <c r="B37" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="300.95">
-      <c r="B38" s="4" t="s">
+    <row r="38" spans="1:4" ht="309" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="14"/>
+      <c r="B38" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="C38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="47.45">
-      <c r="B39" s="4" t="s">
+    <row r="39" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="14"/>
+      <c r="B39" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="C39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="4" t="s">
+    <row r="40" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="14"/>
+      <c r="B40" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="C40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="63.4">
-      <c r="B41" s="4" t="s">
+    <row r="41" spans="1:4" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="14"/>
+      <c r="B41" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="C41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16.5">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:4" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="C42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="79.150000000000006">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:4" ht="92" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="5" t="s">
+      <c r="C43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="C45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5" t="s">
+      <c r="C46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="47.45">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="C48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="47.45">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="C49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="47.45">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="C50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="47.45">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="C51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="47.45">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="C52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="5" t="s">
+      <c r="C53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="C55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16.5">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="C56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16.5">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="15" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16.5">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="5" t="s">
+      <c r="C58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="81">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:5" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="81">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:5" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="5" t="s">
+      <c r="C61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="5" t="s">
+      <c r="C62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="119.85" customHeight="1">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:5" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="C63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="15" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="47.45">
-      <c r="A64" s="3" t="s">
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="C64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="47.45">
-      <c r="A65" s="3" t="s">
+      <c r="C66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="139.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="B67" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="47.45">
-      <c r="A66" s="3" t="s">
+      <c r="C67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B68" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="47.45">
-      <c r="A67" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" s="4" t="s">
+      <c r="C69" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="B70" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="s">
+    </row>
+    <row r="71" spans="1:4" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="4" t="s">
+      <c r="C71" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="5" t="s">
+    </row>
+    <row r="72" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="142.5">
-      <c r="A70" s="3" t="s">
+      <c r="C72" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="D72" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="5" t="s">
+      <c r="C73" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="47.45">
-      <c r="A71" s="3" t="s">
+    <row r="74" spans="1:4" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="D74" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="63.4">
-      <c r="A73" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="47.45">
-      <c r="A74" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="16" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Updated Excel and PDF files for Device UDI
</commit_message>
<xml_diff>
--- a/static/fields/deviceudi_reference.xlsx
+++ b/static/fields/deviceudi_reference.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/59009_icf_com/Documents/Documents/open-fda/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/violet.wren/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{3830A780-073A-4AEF-96B5-7D9CC2E92E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42600800-3E0E-4158-B7EE-FB60B1E866C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078CA254-97C6-B643-BF8B-4AA0D1E87EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_udi_fields" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">device_udi_fields!$C$80</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="156">
   <si>
     <t>Section</t>
   </si>
@@ -368,162 +365,284 @@
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>Device identifiers</t>
-  </si>
-  <si>
     <t>identifiers.id</t>
   </si>
   <si>
-    <t>A unique numeric or alphanumeric code specific to a device version or model.</t>
-  </si>
-  <si>
     <t>identifiers.issuing_agency</t>
   </si>
   <si>
-    <t>Identifies whether facility is an initial importer.
-Value is one of the following
-Y = Yes
-N = No</t>
-  </si>
-  <si>
     <t>identifiers.package_discontinue_date</t>
   </si>
   <si>
-    <t>Year that registration expires (expires 12/31 of that year).</t>
-  </si>
-  <si>
     <t>identifiers.package_status</t>
   </si>
   <si>
-    <t>Facility or US agent address line 1.</t>
-  </si>
-  <si>
-    <t>identifiers.package_type</t>
-  </si>
-  <si>
-    <t>Facility or US agent address line 2.</t>
-  </si>
-  <si>
     <t>identifiers.quantity_per_package</t>
   </si>
   <si>
-    <t>Facility or US agent city.
+    <t>identifiers.type</t>
+  </si>
+  <si>
+    <t>customer_contacts.email</t>
+  </si>
+  <si>
+    <t>customer_contacts.phone</t>
+  </si>
+  <si>
+    <t>Device Size</t>
+  </si>
+  <si>
+    <t>device_sizes.text</t>
+  </si>
+  <si>
+    <t>device_sizes.type</t>
+  </si>
+  <si>
+    <t>Facility identifier assigned to facility by the FDA Office of Regulatory Affairs.</t>
+  </si>
+  <si>
+    <t>device_sizes.value</t>
+  </si>
+  <si>
+    <t>device_sizes.unit</t>
+  </si>
+  <si>
+    <t>gmdn_terms.code</t>
+  </si>
+  <si>
+    <t>gmdn_terms.name</t>
+  </si>
+  <si>
+    <t>gmdn_terms.definition</t>
+  </si>
+  <si>
+    <t>gmdn_terms.implantable</t>
+  </si>
+  <si>
+    <t>gmdn_terms.code_status</t>
+  </si>
+  <si>
+    <t>Premarket Submissions</t>
+  </si>
+  <si>
+    <t>premarket_submissions.submission_number</t>
+  </si>
+  <si>
+    <t>premarket_submissions.supplement_number</t>
+  </si>
+  <si>
+    <t>Number assigned by FDA to a supplemental application for approval of a change in a medical device with an approved PMA.</t>
+  </si>
+  <si>
+    <t>Storage and Handling</t>
+  </si>
+  <si>
+    <t>storage.high.value</t>
+  </si>
+  <si>
+    <t>storage.low.value</t>
+  </si>
+  <si>
+    <t>storage.low.unit</t>
+  </si>
+  <si>
+    <t>storage.special_conditions</t>
+  </si>
+  <si>
+    <t>storage.type</t>
+  </si>
+  <si>
+    <t>OpenFDA fields</t>
+  </si>
+  <si>
+    <t>device_class</t>
+  </si>
+  <si>
+    <t>A risk based classification system for all medical devices ((Federal Food, Drug, and Cosmetic Act, section 513)
+Value is one of the following
+1 = Class I (low to moderate risk): general controls
+2 = Class II (moderate to high risk): general controls and special controls
+3 = Class III (high risk): general controls and Premarket Approval (PMA)
+U = Unclassified
+N = Not classified
+F = HDE</t>
+  </si>
+  <si>
+    <t>device name</t>
+  </si>
+  <si>
+    <t>This is the proprietary name, or trade name, of the cleared device.
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>identifiers.type</t>
-  </si>
-  <si>
-    <t>Facility or US agent US state or foreign state or province.</t>
-  </si>
-  <si>
-    <t>identifiers.unit_of_use_id</t>
-  </si>
-  <si>
-    <t>Number of devices noted in the adverse event report. Almost always 1. May be empty if report_source_code contains Voluntary report.
+    <t>fei_number</t>
+  </si>
+  <si>
+    <t>array of strings</t>
+  </si>
+  <si>
+    <t>medical_specialty_description</t>
+  </si>
+  <si>
+    <t>Regulation Medical Specialty is assigned based on the regulation (e.g. 21 CFR Part 888 is Orthopedic Devices) which is why Class 3 devices lack the “Regulation Medical Specialty” field.
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>Customer Contact</t>
-  </si>
-  <si>
-    <t>customer_contacts.email</t>
-  </si>
-  <si>
-    <t>Facility or US agent Zip code.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>customer_contacts.phone</t>
-  </si>
-  <si>
-    <t>Name associated with the facility or US agent.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>Device Size</t>
-  </si>
-  <si>
-    <t>device_sizes.text</t>
-  </si>
-  <si>
-    <t>Facility foreign postal code.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>device_sizes.type</t>
-  </si>
-  <si>
-    <t>Facility identifier assigned to facility by the FDA Office of Regulatory Affairs.</t>
-  </si>
-  <si>
-    <t>device_sizes.value</t>
-  </si>
-  <si>
-    <t>device_sizes.unit</t>
-  </si>
-  <si>
-    <t>Number assigned to Owner Operator by CDRH.</t>
-  </si>
-  <si>
-    <t>GMDN Terms</t>
-  </si>
-  <si>
-    <t>gmdn_terms.code</t>
-  </si>
-  <si>
-    <t>GMDN Preferred Term Code of the common device type associated with the FDA PT Code.</t>
-  </si>
-  <si>
-    <t>gmdn_terms.name</t>
-  </si>
-  <si>
-    <t>Name of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
-  </si>
-  <si>
-    <t>gmdn_terms.definition</t>
-  </si>
-  <si>
-    <t>Definition of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
-  </si>
-  <si>
-    <t>gmdn_terms.implantable</t>
-  </si>
-  <si>
-    <t>GMDN Implantable flag.
-Value is one of the following
+    <t>regulation_number</t>
+  </si>
+  <si>
+    <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
+  </si>
+  <si>
+    <t>Indicated any special storage requirements for the device.</t>
+  </si>
+  <si>
+    <t>Email for the customer contact; to be used by patients and consumers for device-related questions.</t>
+  </si>
+  <si>
+    <t>Phone number for the customer contact; to be ued by patients and consumers for device-related questions.</t>
+  </si>
+  <si>
+    <t>Additional undefined device size not represented in the GUDID Size Type LOV.</t>
+  </si>
+  <si>
+    <t>Dimension type for the clinically relevant measurement of the medical device.
+Value is one of the following
+Circumference = Circumference
+Depth; Device Size Text, specify = Depth; Device Size Text, specify
+Catheter Gauge= Catheter Gauge
+Outer Diameter: Outer Diameter
+Height = Height
+Length = Length
+Lumen/Inner Diameter = Lumen/Inner Diameter
+Needle Gauge = Needle Gauge
+Total Volume = Total Volume
+Width = Width
+Weight = Weight
+Pressure = Pressure
+Pore Size = Pore Size
+Area/Surface Area = Area/Surface Area
+Angle = Angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The unit of measure associated with each clinically relevant size.
+Value is one of the following
+Centiliter   =   Centiliter  
+Centimeter   =   Centimeter  
+Cubic Inch   =   Cubic Inch  
+Cup   =   Cup  
+Deciliter   =   Deciliter  
+Decimeter   =   Decimeter  
+degree   =   degree  
+ Feet   =   Feet  
+ Femtoliter   =   Femtoliter  
+ Femtometer   =   Femtometer  
+ Fluid Ounce   =   Fluid Ounce  
+ French   =   French  
+ Gallon   =   Gallon  
+ Gauge   =   Gauge  
+ Gram   =   Gram  
+ Hertz   =   Hertz  
+ Inch   =   Inch  
+ Kilogram   =   Kilogram  
+ Kiloliter   =   Kiloliter  
+ Kilometer   =   Kilometer  
+ KiloPascal   =   KiloPascal  
+ Liter   =   Liter  
+ Meter   =   Meter  
+ Microgram   =   Microgram  
+ Microliter   =   Microliter  
+ Micrometer   =   Micrometer  
+ millibar   =   millibar  
+ Milligram   =   Milligram  
+ Milliliter   =   Milliliter  
+ Millimeter   =   Millimeter  
+ Nanoliter   =   Nanoliter  
+ Nanometer   =   Nanometer  
+ Picoliter   =   Picoliter  
+ Picometer   =   Picometer  
+ Pint   =   Pint  
+ Pound   =   Pound  
+ Pound per Square Inch   =   Pound per Square Inch  
+ Quart   =   Quart  
+ Square centimeter   =   Square centimeter  
+ Square foot   =   Square foot  
+ Square inch   =   Square inch  
+ Square meter   =   Square meter  
+ Ton   =   Ton  
+ Yard   =   Yard  </t>
+  </si>
+  <si>
+    <t>Numeric value for the clinically reevant size measurement of the medical device.</t>
+  </si>
+  <si>
+    <t>GMDN preferred term Code of the common device type associated with the FDA PT Code.</t>
+  </si>
+  <si>
+    <t>Definition of the common device type associated with the GMDN Preferred Term Code/FDA PT Code</t>
+  </si>
+  <si>
+    <t>GMDN Implantable flag 
+Value of one of the following:
 true = true
 false = false</t>
   </si>
   <si>
-    <t>gmdn_terms.code_status</t>
-  </si>
-  <si>
-    <t>GMDN Term Status, Active or Obsolete.
-Value is one of the following
+    <t>GMDN  Term Status, Active or Obsolete
+Value of one of the following:
 Active = Active
 Obsolete = Obsolete</t>
   </si>
   <si>
-    <t>Premarket Submissions</t>
-  </si>
-  <si>
-    <t>premarket_submissions.submission_number</t>
-  </si>
-  <si>
-    <t>Number associated with the regulatory decision regarding the applicant’s legal right to market a medical device for the following submission types: 510(k), PMA, PDP, HDE, BLA, and NDA.</t>
-  </si>
-  <si>
-    <t>premarket_submissions.supplement_number</t>
-  </si>
-  <si>
-    <t>Number assigned by FDA to a supplemental application for approval of a change in a medical device with an approved PMA.</t>
-  </si>
-  <si>
-    <t>premarket_submissions.submission_type</t>
-  </si>
-  <si>
-    <t>Indicates the premarket submission type. Value is one of the following
+    <t>A unique numeric or alphanumeric cide specific to a device version or model.</t>
+  </si>
+  <si>
+    <t>Organization accredited by FDA to operate a system for the issuance of UDIs.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
+Value is one of the following
+GS1 = GS1
+ICCBBA = ICCBBA
+HIBCC = HIBCC
+NDC/NHRIC = NDC/NHRIC</t>
+  </si>
+  <si>
+    <t>Indicates the date this particular package configuration is diiscontinued by the Labeler or removed from the marketpace.</t>
+  </si>
+  <si>
+    <t>identifiers.packakage_type</t>
+  </si>
+  <si>
+    <t>The type of packaging used for the device.</t>
+  </si>
+  <si>
+    <t>The number of package with the same Primary DI or Package DI within a given packaging configuration.</t>
+  </si>
+  <si>
+    <t>Indicates whether the identifier is the Primary, Secondary, Direct Marking, Unit of Use, Package, or Previous DI.
+Value is one of the following
+Primary = Primary DI. An identifier that is the main (primary) lookup for a medical device and meets the requirements to uniquely identify a device through its distribution and use.  The primary DI number will be located on the base package, which is the lowest package level of a medical device containing a full UDI.  For medical devices without packaging, the primary DI number and full UDI may be on the device itself."
+Secondary = Secondary DI. An identifier that is an alternate (secondary) lookup for a medical device that is issued from a different issuing agency than the primary DI. Under 21 CFR 830.40(a), only one device identifier from any particular system for the issuance of UDIs may be used to identify a particular version or model of a device.
+Direct Marking = Direct Marking DI. An identifier that is marked directly on the medical device and is different than the Primary DI Number; only applicable to devices subject to Direct Marking requirements under 21 CFR 801.45.
+Unit of Use = Unit of Use DI. An identifier assigned to an individual medical device when a UDI is not labeled on the individual device at the level of its unit of use. Its purpose is to associate the use of a device to/on a patient.
+Package = Package DI. A device identifier for the package configuration that contains multiple units of the base package (does not include shipping containers).
+Previous DI = Previous DI</t>
+  </si>
+  <si>
+    <t>identifiers_unit_od use_id</t>
+  </si>
+  <si>
+    <t>An identifier assigned to an individual medicaldevice when a UDI is not labeled on the individual device at the level of its unit of use. Its purpose is to associate the use of a device to/on a patient. Unit of Use DI is an identifier used by hospital staff and Material amangemnet to account for a single device when the UDI is labeled on a higher level of packaging. The Unit of Use DI does not appear on the label. Data type and field length are determined by the individual Issuing Agency structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number associated with the regulatory decision regarding the applicant’s legal right to market a medical device for the following submission types: 510(k), PMA, PDP, HDE, BLA, and NDA.
+</t>
+  </si>
+  <si>
+    <t>premarket_submission.submission_type</t>
+  </si>
+  <si>
+    <t>Number assigned by FDA to a supplemental application for approval of a change in a medical device with an approved PMA.
+Value is one of the following
 510(k) = 510(k)
 PMA = PMA
 PDP = PDP
@@ -532,98 +651,76 @@
 NDA = NDA</t>
   </si>
   <si>
-    <t>Storage and Handling</t>
-  </si>
-  <si>
-    <t>storage.high.value</t>
-  </si>
-  <si>
-    <t>storage.low.value</t>
-  </si>
-  <si>
-    <t>storage.low.unit</t>
-  </si>
-  <si>
-    <t>storage.special_conditions</t>
-  </si>
-  <si>
-    <t>storage.type</t>
-  </si>
-  <si>
-    <t>OpenFDA fields</t>
-  </si>
-  <si>
-    <t>device_class</t>
-  </si>
-  <si>
-    <t>A risk based classification system for all medical devices ((Federal Food, Drug, and Cosmetic Act, section 513)
-Value is one of the following
-1 = Class I (low to moderate risk): general controls
-2 = Class II (moderate to high risk): general controls and special controls
-3 = Class III (high risk): general controls and Premarket Approval (PMA)
-U = Unclassified
-N = Not classified
-F = HDE</t>
-  </si>
-  <si>
-    <t>device name</t>
-  </si>
-  <si>
-    <t>This is the proprietary name, or trade name, of the cleared device.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>fei_number</t>
-  </si>
-  <si>
-    <t>array of strings</t>
-  </si>
-  <si>
-    <t>medical_specialty_description</t>
-  </si>
-  <si>
-    <t>Regulation Medical Specialty is assigned based on the regulation (e.g. 21 CFR Part 888 is Orthopedic Devices) which is why Class 3 devices lack the “Regulation Medical Specialty” field.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>regulation_number</t>
-  </si>
-  <si>
-    <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
-  </si>
-  <si>
-    <t>Indicates the high value for storage and handling requirements.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>The low value unit of measures associated with the storage and handling conditions.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.eprocessed and reused.</t>
-  </si>
-  <si>
-    <t>Indicates the low value for storage and handling requirements.Value is one of the following
+    <t>GMDN terms</t>
+  </si>
+  <si>
+    <t>Customer Contacts</t>
+  </si>
+  <si>
+    <t>Device Identifiers</t>
+  </si>
+  <si>
+    <t>Product Codes</t>
+  </si>
+  <si>
+    <t>Sterilization</t>
+  </si>
+  <si>
+    <t>storage.high.unit</t>
+  </si>
+  <si>
+    <t>The high value unit of measure associated with the storage and handling conditions.
+Value is one of the following
 Degrees Celsius = Degrees Celsius
 Degrees Fahrenheit = Degrees Fahrenheit
 Degrees Kelvin = Degrees Kelvin
 Kilo Pascal = Kilo Pascal
-Percent (%) Relative Humidity, Millibar = Percent (%) Relative Humidity,Millibar
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized</t>
-  </si>
-  <si>
-    <t>Indicated any special storage requirements for the device.</t>
-  </si>
-  <si>
-    <t>Indicates storage and handling requirements for the device inclusing temperature, humidity, and atmospheric pressure.</t>
-  </si>
-  <si>
-    <t>The high value unit of measure associated with the storage and handling conditions.
+Percent (%) Relative Humidity, Millibar = Percent (%) Relative Humidity,Millibar</t>
+  </si>
+  <si>
+    <t>Indicates the high value for storage and handling requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low value unit of measures associated with the storage and handling conditions.
+</t>
+  </si>
+  <si>
+    <t>Indicates the low value for storage and handling requirements
+Value is one of the following
+Degrees Celsius = Degrees Celsius
+Degrees Fahrenheit = Degrees Fahrenheit
+Degrees Kelvin = Degrees Kelvin
+Kilo Pascal = Kilo Pascal
+Percent (%) Relative Humidity, Millibar = Percent (%) Relative Humidity,Millibar</t>
+  </si>
+  <si>
+    <t>Indicates storage and handling requirements for the device including temperature, humidity, and atmospheric pressure.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
+Handling Environment Atmospheric Pressure = Handling Environment Atmospheric Pressure
+Handling Environment Humidity = Handling Environment Humidity
+Handling Environment Temperature = Handling Environment Temperature
+Special Storage Conditions = Special Storage Conditions
+Storage Environment Atmospheric Pressure = Storage Environment Atmospheric Pressure
+Storage Environment Humidity = Storage Environment Humidity
+Storage Environment Temperature = Storage Environment Temperature</t>
+  </si>
+  <si>
+    <t>Name of the common device type associated with the GMDN Preferred Term Code/ FDA PT Code..
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>Indicates whether the package is in commercial distribution as defined under 21 CFR 807.3(b)
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
+Value is one of the following
+In Commercial Distribution = In Commercial Distribution
+Not in Commercial Distribution = Not in Commercial Distribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,13 +758,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -677,7 +767,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -701,11 +791,43 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -720,7 +842,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -732,12 +854,64 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -747,27 +921,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -780,55 +937,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1109,7 +1219,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1123,50 +1233,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="273">
@@ -1455,10 +1574,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1783,963 +1898,954 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B70" sqref="A34:D74"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.33203125" style="3" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="6" t="s">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="145.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="133.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
-      <c r="B10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="139.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="6" t="s">
-        <v>26</v>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="6" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="340" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="6" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="131.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="6" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="98" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>5</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="6" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="6" t="s">
-        <v>38</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="6" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="6" t="s">
-        <v>42</v>
+      <c r="D18" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="98.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="6" t="s">
-        <v>44</v>
+      <c r="D19" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
-      <c r="B21" s="6" t="s">
-        <v>46</v>
+      <c r="D20" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="6" t="s">
-        <v>48</v>
+      <c r="D21" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="6" t="s">
-        <v>50</v>
+      <c r="D22" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
+      <c r="D23" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="175" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="6" t="s">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="6" t="s">
-        <v>56</v>
+      <c r="D25" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="6" t="s">
-        <v>58</v>
+      <c r="D27" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
-      <c r="B30" s="6" t="s">
-        <v>60</v>
+      <c r="D28" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="15"/>
-    </row>
-    <row r="32" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
-      <c r="B32" s="6" t="s">
-        <v>62</v>
+        <v>17</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="15"/>
-    </row>
-    <row r="34" spans="1:4" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
-      <c r="B34" s="6" t="s">
-        <v>64</v>
+        <v>5</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="B34" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="93" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
-      <c r="B35" s="6" t="s">
-        <v>66</v>
+        <v>22</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
-      <c r="B36" s="6" t="s">
-        <v>68</v>
+        <v>22</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
-      <c r="B37" s="6" t="s">
-        <v>70</v>
+      <c r="D36" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="309" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="14"/>
-      <c r="B38" s="6" t="s">
-        <v>72</v>
+      <c r="D37" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
-      <c r="B39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="15" t="s">
+      <c r="C48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="14"/>
-      <c r="B40" s="6" t="s">
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="15" t="s">
+      <c r="C49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="4" t="s">
+    <row r="50" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="22" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="17"/>
+      <c r="B54" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>108</v>
+      <c r="D54" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="11"/>
+      <c r="B55" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>111</v>
+        <v>10</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" s="11"/>
+      <c r="B56" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>113</v>
+      <c r="D56" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="11"/>
+      <c r="B57" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>115</v>
+      <c r="D57" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A58" s="11"/>
+      <c r="B58" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>117</v>
+      <c r="D58" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A59" s="11"/>
+      <c r="B59" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>119</v>
+        <v>5</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="139.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>132</v>
+    <row r="68" spans="1:4" ht="340" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>133</v>
+      <c r="D68" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A69" s="11"/>
+      <c r="B69" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D69" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>135</v>
+      <c r="D69" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>144</v>
+        <v>115</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{cf90b97b-be46-4a00-9700-81ce4ff1b7f6}" enabled="0" method="" siteId="{cf90b97b-be46-4a00-9700-81ce4ff1b7f6}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
UDI Searchable Fields Reference Document updated (#296)
* UDI Searchable Fields Reference Document updated

* Updated Excel and PDF files for Device UDI

* Removed fei_number

* Usage update - 10/25

---------

Co-authored-by: Ayer <59009@icf.com>
Co-authored-by: violet.wren <violet.wren@semanticbits.com>
</commit_message>
<xml_diff>
--- a/static/fields/deviceudi_reference.xlsx
+++ b/static/fields/deviceudi_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/violet.wren/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3830A780-073A-4AEF-96B5-7D9CC2E92E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015BB07A-E326-8546-B966-1983E5A2F056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1003" yWindow="0" windowWidth="23455" windowHeight="12485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_udi_fields" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="154">
   <si>
     <t>Section</t>
   </si>
@@ -365,162 +365,278 @@
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>Device identifiers</t>
-  </si>
-  <si>
     <t>identifiers.id</t>
   </si>
   <si>
-    <t>A unique numeric or alphanumeric code specific to a device version or model.</t>
-  </si>
-  <si>
     <t>identifiers.issuing_agency</t>
   </si>
   <si>
-    <t>Identifies whether facility is an initial importer.
-Value is one of the following
-Y = Yes
-N = No</t>
-  </si>
-  <si>
     <t>identifiers.package_discontinue_date</t>
   </si>
   <si>
-    <t>Year that registration expires (expires 12/31 of that year).</t>
-  </si>
-  <si>
     <t>identifiers.package_status</t>
   </si>
   <si>
-    <t>Facility or US agent address line 1.</t>
-  </si>
-  <si>
-    <t>identifiers.package_type</t>
-  </si>
-  <si>
-    <t>Facility or US agent address line 2.</t>
-  </si>
-  <si>
     <t>identifiers.quantity_per_package</t>
   </si>
   <si>
-    <t>Facility or US agent city.
+    <t>identifiers.type</t>
+  </si>
+  <si>
+    <t>customer_contacts.email</t>
+  </si>
+  <si>
+    <t>customer_contacts.phone</t>
+  </si>
+  <si>
+    <t>Device Size</t>
+  </si>
+  <si>
+    <t>device_sizes.text</t>
+  </si>
+  <si>
+    <t>device_sizes.type</t>
+  </si>
+  <si>
+    <t>device_sizes.value</t>
+  </si>
+  <si>
+    <t>device_sizes.unit</t>
+  </si>
+  <si>
+    <t>gmdn_terms.code</t>
+  </si>
+  <si>
+    <t>gmdn_terms.name</t>
+  </si>
+  <si>
+    <t>gmdn_terms.definition</t>
+  </si>
+  <si>
+    <t>gmdn_terms.implantable</t>
+  </si>
+  <si>
+    <t>gmdn_terms.code_status</t>
+  </si>
+  <si>
+    <t>Premarket Submissions</t>
+  </si>
+  <si>
+    <t>premarket_submissions.submission_number</t>
+  </si>
+  <si>
+    <t>premarket_submissions.supplement_number</t>
+  </si>
+  <si>
+    <t>Number assigned by FDA to a supplemental application for approval of a change in a medical device with an approved PMA.</t>
+  </si>
+  <si>
+    <t>Storage and Handling</t>
+  </si>
+  <si>
+    <t>storage.high.value</t>
+  </si>
+  <si>
+    <t>storage.low.value</t>
+  </si>
+  <si>
+    <t>storage.low.unit</t>
+  </si>
+  <si>
+    <t>storage.special_conditions</t>
+  </si>
+  <si>
+    <t>storage.type</t>
+  </si>
+  <si>
+    <t>OpenFDA fields</t>
+  </si>
+  <si>
+    <t>device_class</t>
+  </si>
+  <si>
+    <t>A risk based classification system for all medical devices ((Federal Food, Drug, and Cosmetic Act, section 513)
+Value is one of the following
+1 = Class I (low to moderate risk): general controls
+2 = Class II (moderate to high risk): general controls and special controls
+3 = Class III (high risk): general controls and Premarket Approval (PMA)
+U = Unclassified
+N = Not classified
+F = HDE</t>
+  </si>
+  <si>
+    <t>device name</t>
+  </si>
+  <si>
+    <t>This is the proprietary name, or trade name, of the cleared device.
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>identifiers.type</t>
-  </si>
-  <si>
-    <t>Facility or US agent US state or foreign state or province.</t>
-  </si>
-  <si>
-    <t>identifiers.unit_of_use_id</t>
-  </si>
-  <si>
-    <t>Number of devices noted in the adverse event report. Almost always 1. May be empty if report_source_code contains Voluntary report.
+    <t>array of strings</t>
+  </si>
+  <si>
+    <t>medical_specialty_description</t>
+  </si>
+  <si>
+    <t>Regulation Medical Specialty is assigned based on the regulation (e.g. 21 CFR Part 888 is Orthopedic Devices) which is why Class 3 devices lack the “Regulation Medical Specialty” field.
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>Customer Contact</t>
-  </si>
-  <si>
-    <t>customer_contacts.email</t>
-  </si>
-  <si>
-    <t>Facility or US agent Zip code.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>customer_contacts.phone</t>
-  </si>
-  <si>
-    <t>Name associated with the facility or US agent.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>Device Size</t>
-  </si>
-  <si>
-    <t>device_sizes.text</t>
-  </si>
-  <si>
-    <t>Facility foreign postal code.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>device_sizes.type</t>
-  </si>
-  <si>
-    <t>Facility identifier assigned to facility by the FDA Office of Regulatory Affairs.</t>
-  </si>
-  <si>
-    <t>device_sizes.value</t>
-  </si>
-  <si>
-    <t>device_sizes.unit</t>
-  </si>
-  <si>
-    <t>Number assigned to Owner Operator by CDRH.</t>
-  </si>
-  <si>
-    <t>GMDN Terms</t>
-  </si>
-  <si>
-    <t>gmdn_terms.code</t>
-  </si>
-  <si>
-    <t>GMDN Preferred Term Code of the common device type associated with the FDA PT Code.</t>
-  </si>
-  <si>
-    <t>gmdn_terms.name</t>
-  </si>
-  <si>
-    <t>Name of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
-  </si>
-  <si>
-    <t>gmdn_terms.definition</t>
-  </si>
-  <si>
-    <t>Definition of the common device type associated with the GMDN Preferred Term Code/FDA PT Code.</t>
-  </si>
-  <si>
-    <t>gmdn_terms.implantable</t>
-  </si>
-  <si>
-    <t>GMDN Implantable flag.
-Value is one of the following
+    <t>regulation_number</t>
+  </si>
+  <si>
+    <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
+  </si>
+  <si>
+    <t>Indicated any special storage requirements for the device.</t>
+  </si>
+  <si>
+    <t>Email for the customer contact; to be used by patients and consumers for device-related questions.</t>
+  </si>
+  <si>
+    <t>Phone number for the customer contact; to be ued by patients and consumers for device-related questions.</t>
+  </si>
+  <si>
+    <t>Additional undefined device size not represented in the GUDID Size Type LOV.</t>
+  </si>
+  <si>
+    <t>Dimension type for the clinically relevant measurement of the medical device.
+Value is one of the following
+Circumference = Circumference
+Depth; Device Size Text, specify = Depth; Device Size Text, specify
+Catheter Gauge= Catheter Gauge
+Outer Diameter: Outer Diameter
+Height = Height
+Length = Length
+Lumen/Inner Diameter = Lumen/Inner Diameter
+Needle Gauge = Needle Gauge
+Total Volume = Total Volume
+Width = Width
+Weight = Weight
+Pressure = Pressure
+Pore Size = Pore Size
+Area/Surface Area = Area/Surface Area
+Angle = Angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The unit of measure associated with each clinically relevant size.
+Value is one of the following
+Centiliter   =   Centiliter  
+Centimeter   =   Centimeter  
+Cubic Inch   =   Cubic Inch  
+Cup   =   Cup  
+Deciliter   =   Deciliter  
+Decimeter   =   Decimeter  
+degree   =   degree  
+ Feet   =   Feet  
+ Femtoliter   =   Femtoliter  
+ Femtometer   =   Femtometer  
+ Fluid Ounce   =   Fluid Ounce  
+ French   =   French  
+ Gallon   =   Gallon  
+ Gauge   =   Gauge  
+ Gram   =   Gram  
+ Hertz   =   Hertz  
+ Inch   =   Inch  
+ Kilogram   =   Kilogram  
+ Kiloliter   =   Kiloliter  
+ Kilometer   =   Kilometer  
+ KiloPascal   =   KiloPascal  
+ Liter   =   Liter  
+ Meter   =   Meter  
+ Microgram   =   Microgram  
+ Microliter   =   Microliter  
+ Micrometer   =   Micrometer  
+ millibar   =   millibar  
+ Milligram   =   Milligram  
+ Milliliter   =   Milliliter  
+ Millimeter   =   Millimeter  
+ Nanoliter   =   Nanoliter  
+ Nanometer   =   Nanometer  
+ Picoliter   =   Picoliter  
+ Picometer   =   Picometer  
+ Pint   =   Pint  
+ Pound   =   Pound  
+ Pound per Square Inch   =   Pound per Square Inch  
+ Quart   =   Quart  
+ Square centimeter   =   Square centimeter  
+ Square foot   =   Square foot  
+ Square inch   =   Square inch  
+ Square meter   =   Square meter  
+ Ton   =   Ton  
+ Yard   =   Yard  </t>
+  </si>
+  <si>
+    <t>Numeric value for the clinically reevant size measurement of the medical device.</t>
+  </si>
+  <si>
+    <t>GMDN preferred term Code of the common device type associated with the FDA PT Code.</t>
+  </si>
+  <si>
+    <t>Definition of the common device type associated with the GMDN Preferred Term Code/FDA PT Code</t>
+  </si>
+  <si>
+    <t>GMDN Implantable flag 
+Value of one of the following:
 true = true
 false = false</t>
   </si>
   <si>
-    <t>gmdn_terms.code_status</t>
-  </si>
-  <si>
-    <t>GMDN Term Status, Active or Obsolete.
-Value is one of the following
+    <t>GMDN  Term Status, Active or Obsolete
+Value of one of the following:
 Active = Active
 Obsolete = Obsolete</t>
   </si>
   <si>
-    <t>Premarket Submissions</t>
-  </si>
-  <si>
-    <t>premarket_submissions.submission_number</t>
-  </si>
-  <si>
-    <t>Number associated with the regulatory decision regarding the applicant’s legal right to market a medical device for the following submission types: 510(k), PMA, PDP, HDE, BLA, and NDA.</t>
-  </si>
-  <si>
-    <t>premarket_submissions.supplement_number</t>
-  </si>
-  <si>
-    <t>Number assigned by FDA to a supplemental application for approval of a change in a medical device with an approved PMA.</t>
-  </si>
-  <si>
-    <t>premarket_submissions.submission_type</t>
-  </si>
-  <si>
-    <t>Indicates the premarket submission type. Value is one of the following
+    <t>A unique numeric or alphanumeric cide specific to a device version or model.</t>
+  </si>
+  <si>
+    <t>Organization accredited by FDA to operate a system for the issuance of UDIs.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
+Value is one of the following
+GS1 = GS1
+ICCBBA = ICCBBA
+HIBCC = HIBCC
+NDC/NHRIC = NDC/NHRIC</t>
+  </si>
+  <si>
+    <t>Indicates the date this particular package configuration is diiscontinued by the Labeler or removed from the marketpace.</t>
+  </si>
+  <si>
+    <t>identifiers.packakage_type</t>
+  </si>
+  <si>
+    <t>The type of packaging used for the device.</t>
+  </si>
+  <si>
+    <t>The number of package with the same Primary DI or Package DI within a given packaging configuration.</t>
+  </si>
+  <si>
+    <t>Indicates whether the identifier is the Primary, Secondary, Direct Marking, Unit of Use, Package, or Previous DI.
+Value is one of the following
+Primary = Primary DI. An identifier that is the main (primary) lookup for a medical device and meets the requirements to uniquely identify a device through its distribution and use.  The primary DI number will be located on the base package, which is the lowest package level of a medical device containing a full UDI.  For medical devices without packaging, the primary DI number and full UDI may be on the device itself."
+Secondary = Secondary DI. An identifier that is an alternate (secondary) lookup for a medical device that is issued from a different issuing agency than the primary DI. Under 21 CFR 830.40(a), only one device identifier from any particular system for the issuance of UDIs may be used to identify a particular version or model of a device.
+Direct Marking = Direct Marking DI. An identifier that is marked directly on the medical device and is different than the Primary DI Number; only applicable to devices subject to Direct Marking requirements under 21 CFR 801.45.
+Unit of Use = Unit of Use DI. An identifier assigned to an individual medical device when a UDI is not labeled on the individual device at the level of its unit of use. Its purpose is to associate the use of a device to/on a patient.
+Package = Package DI. A device identifier for the package configuration that contains multiple units of the base package (does not include shipping containers).
+Previous DI = Previous DI</t>
+  </si>
+  <si>
+    <t>identifiers_unit_od use_id</t>
+  </si>
+  <si>
+    <t>An identifier assigned to an individual medicaldevice when a UDI is not labeled on the individual device at the level of its unit of use. Its purpose is to associate the use of a device to/on a patient. Unit of Use DI is an identifier used by hospital staff and Material amangemnet to account for a single device when the UDI is labeled on a higher level of packaging. The Unit of Use DI does not appear on the label. Data type and field length are determined by the individual Issuing Agency structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number associated with the regulatory decision regarding the applicant’s legal right to market a medical device for the following submission types: 510(k), PMA, PDP, HDE, BLA, and NDA.
+</t>
+  </si>
+  <si>
+    <t>premarket_submission.submission_type</t>
+  </si>
+  <si>
+    <t>Number assigned by FDA to a supplemental application for approval of a change in a medical device with an approved PMA.
+Value is one of the following
 510(k) = 510(k)
 PMA = PMA
 PDP = PDP
@@ -529,93 +645,76 @@
 NDA = NDA</t>
   </si>
   <si>
-    <t>Storage and Handling</t>
-  </si>
-  <si>
-    <t>storage.high.value</t>
-  </si>
-  <si>
-    <t>Official correspondent last name.
+    <t>GMDN terms</t>
+  </si>
+  <si>
+    <t>Customer Contacts</t>
+  </si>
+  <si>
+    <t>Device Identifiers</t>
+  </si>
+  <si>
+    <t>Product Codes</t>
+  </si>
+  <si>
+    <t>Sterilization</t>
+  </si>
+  <si>
+    <t>storage.high.unit</t>
+  </si>
+  <si>
+    <t>The high value unit of measure associated with the storage and handling conditions.
+Value is one of the following
+Degrees Celsius = Degrees Celsius
+Degrees Fahrenheit = Degrees Fahrenheit
+Degrees Kelvin = Degrees Kelvin
+Kilo Pascal = Kilo Pascal
+Percent (%) Relative Humidity, Millibar = Percent (%) Relative Humidity,Millibar</t>
+  </si>
+  <si>
+    <t>Indicates the high value for storage and handling requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low value unit of measures associated with the storage and handling conditions.
+</t>
+  </si>
+  <si>
+    <t>Indicates the low value for storage and handling requirements
+Value is one of the following
+Degrees Celsius = Degrees Celsius
+Degrees Fahrenheit = Degrees Fahrenheit
+Degrees Kelvin = Degrees Kelvin
+Kilo Pascal = Kilo Pascal
+Percent (%) Relative Humidity, Millibar = Percent (%) Relative Humidity,Millibar</t>
+  </si>
+  <si>
+    <t>Indicates storage and handling requirements for the device including temperature, humidity, and atmospheric pressure.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
+Handling Environment Atmospheric Pressure = Handling Environment Atmospheric Pressure
+Handling Environment Humidity = Handling Environment Humidity
+Handling Environment Temperature = Handling Environment Temperature
+Special Storage Conditions = Special Storage Conditions
+Storage Environment Atmospheric Pressure = Storage Environment Atmospheric Pressure
+Storage Environment Humidity = Storage Environment Humidity
+Storage Environment Temperature = Storage Environment Temperature</t>
+  </si>
+  <si>
+    <t>Name of the common device type associated with the GMDN Preferred Term Code/ FDA PT Code..
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>Official correspondent middle initial.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>storage.low.value</t>
-  </si>
-  <si>
-    <t>Official correspondent phone number.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.eprocessed and reused.</t>
-  </si>
-  <si>
-    <t>storage.low.unit</t>
-  </si>
-  <si>
-    <t>Official correspondent company name (if different from owner operator company name).
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>storage.special_conditions</t>
-  </si>
-  <si>
-    <t>First line of address for owner operator.</t>
-  </si>
-  <si>
-    <t>storage.type</t>
-  </si>
-  <si>
-    <t>Second line of address for owner operator.</t>
-  </si>
-  <si>
-    <t>OpenFDA fields</t>
-  </si>
-  <si>
-    <t>device_class</t>
-  </si>
-  <si>
-    <t>A risk based classification system for all medical devices ((Federal Food, Drug, and Cosmetic Act, section 513)
-Value is one of the following
-1 = Class I (low to moderate risk): general controls
-2 = Class II (moderate to high risk): general controls and special controls
-3 = Class III (high risk): general controls and Premarket Approval (PMA)
-U = Unclassified
-N = Not classified
-F = HDE</t>
-  </si>
-  <si>
-    <t>device name</t>
-  </si>
-  <si>
-    <t>This is the proprietary name, or trade name, of the cleared device.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>fei_number</t>
-  </si>
-  <si>
-    <t>array of strings</t>
-  </si>
-  <si>
-    <t>medical_specialty_description</t>
-  </si>
-  <si>
-    <t>Regulation Medical Specialty is assigned based on the regulation (e.g. 21 CFR Part 888 is Orthopedic Devices) which is why Class 3 devices lack the “Regulation Medical Specialty” field.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>regulation_number</t>
-  </si>
-  <si>
-    <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
+    <t>Indicates whether the package is in commercial distribution as defined under 21 CFR 807.3(b)
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
+Value is one of the following
+In Commercial Distribution = In Commercial Distribution
+Not in Commercial Distribution = Not in Commercial Distribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -653,13 +752,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -669,7 +761,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -677,6 +769,174 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -953,14 +1213,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -970,17 +1224,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="273">
@@ -1593,902 +1889,940 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="3"/>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="79.150000000000006">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.45">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.7">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="110.85">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.45">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="4" t="s">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="126.75">
-      <c r="B9" s="4" t="s">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="340" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D20" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="110.85">
-      <c r="B10" s="4" t="s">
+    <row r="21" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D21" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="126.75">
-      <c r="B11" s="4" t="s">
+    <row r="22" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D22" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="110.85">
-      <c r="B12" s="4" t="s">
+    <row r="23" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D23" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="110.85">
-      <c r="B13" s="4" t="s">
+    <row r="24" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D24" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="110.85">
-      <c r="B14" s="4" t="s">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D33" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="79.150000000000006">
-      <c r="B15" s="4" t="s">
+    <row r="34" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="B34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D34" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="95.1">
-      <c r="B16" s="4" t="s">
+    <row r="35" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D35" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="95.1">
-      <c r="B17" s="4" t="s">
+    <row r="36" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D36" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="110.85">
-      <c r="B18" s="4" t="s">
+    <row r="37" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D37" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="126.75">
-      <c r="B19" s="4" t="s">
+    <row r="38" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D38" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="79.150000000000006">
-      <c r="B20" s="4" t="s">
+    <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D39" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="79.150000000000006">
-      <c r="B21" s="4" t="s">
+    <row r="40" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D40" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="79.150000000000006">
-      <c r="B22" s="4" t="s">
+    <row r="41" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D41" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="79.150000000000006">
-      <c r="B23" s="4" t="s">
+    <row r="42" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D42" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="31.7">
-      <c r="B24" s="4" t="s">
+    <row r="43" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="C43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="158.44999999999999">
-      <c r="B25" s="4" t="s">
+    <row r="44" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="C44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="31.7">
-      <c r="B26" s="4" t="s">
+    <row r="45" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="17"/>
+      <c r="B54" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="11"/>
+      <c r="B55" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C55" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D55" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="4" t="s">
+    <row r="56" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" s="11"/>
+      <c r="B56" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="C56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="4" t="s">
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="11"/>
+      <c r="B57" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="43.7" customHeight="1">
-      <c r="B34" s="4" t="s">
+    <row r="58" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A58" s="11"/>
+      <c r="B58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="C58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="95.1">
-      <c r="B35" s="4" t="s">
+    <row r="59" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A59" s="11"/>
+      <c r="B59" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="81">
-      <c r="B36" s="4" t="s">
+    <row r="60" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C60" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D60" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="79.150000000000006">
-      <c r="B37" s="4" t="s">
+    <row r="61" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C61" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D61" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="300.95">
-      <c r="B38" s="4" t="s">
+    <row r="62" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="C62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="47.45">
-      <c r="B39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="63.4">
-      <c r="B41" s="4" t="s">
+    <row r="63" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="340" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A69" s="11"/>
+      <c r="B69" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="C69" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16.5">
-      <c r="A42" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="79.150000000000006">
-      <c r="A43" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="47.45">
-      <c r="A47" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="47.45">
-      <c r="A49" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="47.45">
-      <c r="A50" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="47.45">
-      <c r="A51" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="47.45">
-      <c r="A52" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="16.5">
-      <c r="A56" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="16.5">
-      <c r="A57" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="16.5">
-      <c r="A58" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="81">
-      <c r="A59" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="81">
-      <c r="A60" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="119.85" customHeight="1">
-      <c r="A63" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="47.45">
-      <c r="A64" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="47.45">
-      <c r="A65" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="47.45">
-      <c r="A66" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="47.45">
-      <c r="A67" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="142.5">
-      <c r="A70" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="47.45">
-      <c r="A71" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="63.4">
-      <c r="A73" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="47.45">
-      <c r="A74" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="16" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{cf90b97b-be46-4a00-9700-81ce4ff1b7f6}" enabled="0" method="" siteId="{cf90b97b-be46-4a00-9700-81ce4ff1b7f6}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>